<commit_message>
branch and bound algorithm implemented
</commit_message>
<xml_diff>
--- a/amod-scheduling/dataset/instances.xlsx
+++ b/amod-scheduling/dataset/instances.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pacio/Desktop/untitled folder 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carmi\Documents\Universita\2 magistrale\2° semestre\AMOD\Progetto\amod-scheduling\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{85098940-5ECD-4FBF-8181-5D56425FDE6E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="27315" windowHeight="14895" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -52,9 +53,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -82,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -93,15 +102,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -369,16 +382,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,7 +411,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -409,132 +422,68 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
         <v>5</v>
-      </c>
-      <c r="B8">
-        <v>89</v>
-      </c>
-      <c r="C8">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>58</v>
-      </c>
-      <c r="C9">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>85</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>54</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>71</v>
-      </c>
-      <c r="C12">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>45</v>
-      </c>
-      <c r="C13">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +503,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -565,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -576,7 +525,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -587,7 +536,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -598,7 +547,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -609,7 +558,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -620,7 +569,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -631,7 +580,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -642,7 +591,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -653,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -664,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -675,7 +624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -686,7 +635,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -697,7 +646,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -708,7 +657,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -719,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -730,7 +679,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -741,7 +690,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -752,7 +701,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -763,7 +712,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -774,7 +723,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -785,7 +734,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -796,7 +745,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -807,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -818,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -829,7 +778,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -840,7 +789,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -851,7 +800,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -862,7 +811,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -873,7 +822,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -884,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -901,16 +850,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +879,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -941,7 +890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -952,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -963,7 +912,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -974,7 +923,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -985,7 +934,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -996,7 +945,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1007,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1018,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1029,7 +978,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1040,7 +989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1051,7 +1000,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1062,7 +1011,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1073,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1084,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1095,7 +1044,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1106,7 +1055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1117,7 +1066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1128,7 +1077,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1139,7 +1088,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1150,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1161,7 +1110,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1172,7 +1121,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1183,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1194,7 +1143,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1205,7 +1154,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1216,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1227,7 +1176,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1238,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1249,7 +1198,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1260,7 +1209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1277,16 +1226,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1306,7 +1255,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1317,7 +1266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1328,7 +1277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1339,7 +1288,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1350,7 +1299,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1361,7 +1310,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1372,7 +1321,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1383,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1394,7 +1343,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1405,7 +1354,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1416,7 +1365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1427,7 +1376,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1438,7 +1387,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1449,7 +1398,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1460,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1471,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1482,7 +1431,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1493,7 +1442,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1504,7 +1453,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1515,7 +1464,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1526,7 +1475,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1537,7 +1486,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1548,7 +1497,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1559,7 +1508,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1570,7 +1519,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1581,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1592,7 +1541,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1603,7 +1552,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1614,7 +1563,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1625,7 +1574,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1636,7 +1585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1647,7 +1596,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1658,7 +1607,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1669,7 +1618,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -1680,7 +1629,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -1691,7 +1640,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -1702,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -1713,7 +1662,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -1724,7 +1673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -1735,7 +1684,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -1746,7 +1695,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -1763,16 +1712,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1803,7 +1752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1814,7 +1763,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1825,7 +1774,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1836,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1847,7 +1796,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1858,7 +1807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1869,7 +1818,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1880,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1891,7 +1840,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1902,7 +1851,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1913,7 +1862,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1924,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1935,7 +1884,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1946,7 +1895,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1957,7 +1906,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1968,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -1979,7 +1928,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1990,7 +1939,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2001,7 +1950,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2012,7 +1961,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2023,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2034,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2045,7 +1994,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2056,7 +2005,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2067,7 +2016,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2078,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2089,7 +2038,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2100,7 +2049,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2111,7 +2060,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2122,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2133,7 +2082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2144,7 +2093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2155,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2166,7 +2115,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2177,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2188,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2199,7 +2148,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2210,7 +2159,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2221,7 +2170,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2232,7 +2181,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2249,16 +2198,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2278,7 +2227,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2289,7 +2238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2300,7 +2249,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2311,7 +2260,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2322,7 +2271,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2333,7 +2282,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2344,7 +2293,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2355,7 +2304,7 @@
         <v>2084</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2366,7 +2315,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2377,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2388,7 +2337,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2399,7 +2348,7 @@
         <v>2241</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2410,7 +2359,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2421,7 +2370,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -2432,7 +2381,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2443,7 +2392,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2454,7 +2403,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2465,7 +2414,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2476,7 +2425,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2487,7 +2436,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2498,7 +2447,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2509,7 +2458,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2520,7 +2469,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2531,7 +2480,7 @@
         <v>2798</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2542,7 +2491,7 @@
         <v>2343</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2553,7 +2502,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2564,7 +2513,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2575,7 +2524,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2586,7 +2535,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2597,7 +2546,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2608,7 +2557,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2619,7 +2568,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2630,7 +2579,7 @@
         <v>2383</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2641,7 +2590,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2652,7 +2601,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2663,7 +2612,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2674,7 +2623,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2685,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2696,7 +2645,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2707,7 +2656,7 @@
         <v>1855</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2718,7 +2667,7 @@
         <v>2822</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2729,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
@@ -2740,7 +2689,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2751,7 +2700,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2762,7 +2711,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
@@ -2773,7 +2722,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
@@ -2784,7 +2733,7 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -2795,7 +2744,7 @@
         <v>2778</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -2806,7 +2755,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
@@ -2817,7 +2766,7 @@
         <v>2358</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
@@ -2828,7 +2777,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -2839,7 +2788,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -2850,7 +2799,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
@@ -2861,7 +2810,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -2872,7 +2821,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -2883,7 +2832,7 @@
         <v>2193</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -2894,7 +2843,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
@@ -2905,7 +2854,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
@@ -2916,7 +2865,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
@@ -2927,7 +2876,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
@@ -2938,7 +2887,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>

</xml_diff>